<commit_message>
Retestando a criacao de tabela
</commit_message>
<xml_diff>
--- a/IMDB Movie Ratings.xlsx
+++ b/IMDB Movie Ratings.xlsx
@@ -615,7 +615,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>8.9</t>
+          <t>8.8</t>
         </is>
       </c>
     </row>
@@ -1287,12 +1287,12 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Os Suspeitos</t>
+          <t>Os Infiltrados</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>1995</t>
+          <t>2006</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
@@ -1309,12 +1309,12 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Os Infiltrados</t>
+          <t>Os Suspeitos</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>2006</t>
+          <t>1995</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
@@ -1397,12 +1397,12 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Top Gun: Maverick</t>
+          <t>Intocáveis</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>2022</t>
+          <t>2011</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
@@ -1419,12 +1419,12 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Intocáveis</t>
+          <t>Túmulo dos Vagalumes</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>2011</t>
+          <t>1988</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
@@ -1441,17 +1441,17 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Tempos Modernos</t>
+          <t>Harakiri</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>1936</t>
+          <t>1962</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>8.4</t>
+          <t>8.5</t>
         </is>
       </c>
     </row>
@@ -1463,12 +1463,12 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Harakiri</t>
+          <t>Tempos Modernos</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>1962</t>
+          <t>1936</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
@@ -1485,12 +1485,12 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Túmulo dos Vagalumes</t>
+          <t>Era uma Vez no Oeste</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>1988</t>
+          <t>1968</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
@@ -1507,12 +1507,12 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Era uma Vez no Oeste</t>
+          <t>Janela Indiscreta</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>1968</t>
+          <t>1954</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
@@ -1529,12 +1529,12 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Janela Indiscreta</t>
+          <t>Alien - O 8º Passageiro</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>1954</t>
+          <t>1979</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
@@ -1551,12 +1551,12 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Alien - O 8º Passageiro</t>
+          <t>Luzes da Cidade</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>1979</t>
+          <t>1931</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
@@ -1573,12 +1573,12 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Luzes da Cidade</t>
+          <t>Cinema Paradiso</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>1931</t>
+          <t>1988</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
@@ -1595,12 +1595,12 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Cinema Paradiso</t>
+          <t>Apocalypse Now</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>1988</t>
+          <t>1979</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
@@ -1639,12 +1639,12 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Apocalypse Now</t>
+          <t>Os Caçadores da Arca Perdida</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>1979</t>
+          <t>1981</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
@@ -1661,12 +1661,12 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Os Caçadores da Arca Perdida</t>
+          <t>Django Livre</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>1981</t>
+          <t>2012</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
@@ -1683,12 +1683,12 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Django Livre</t>
+          <t>WALL·E</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>2012</t>
+          <t>2008</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
@@ -1705,12 +1705,12 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>WALL·E</t>
+          <t>A Vida dos Outros</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>2008</t>
+          <t>2006</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
@@ -1727,12 +1727,12 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>A Vida dos Outros</t>
+          <t>Crepúsculo dos Deuses</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>2006</t>
+          <t>1950</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
@@ -1749,12 +1749,12 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Crepúsculo dos Deuses</t>
+          <t>Glória Feita de Sangue</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>1950</t>
+          <t>1957</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
@@ -1771,12 +1771,12 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Glória Feita de Sangue</t>
+          <t>O Iluminado</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>1957</t>
+          <t>1980</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
@@ -1793,12 +1793,12 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>O Iluminado</t>
+          <t>O Grande Ditador</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>1980</t>
+          <t>1940</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
@@ -1815,12 +1815,12 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>O Grande Ditador</t>
+          <t>Vingadores: Guerra Infinita</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>1940</t>
+          <t>2018</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
@@ -1859,17 +1859,17 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Vingadores: Guerra Infinita</t>
+          <t>Top Gun: Maverick</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>2018</t>
+          <t>2022</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>8.4</t>
+          <t>8.3</t>
         </is>
       </c>
     </row>
@@ -2035,12 +2035,12 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>Coração Valente</t>
+          <t>Amadeus</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>1995</t>
+          <t>1984</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
@@ -2057,12 +2057,12 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>Amadeus</t>
+          <t>Coração Valente</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>1984</t>
+          <t>1995</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
@@ -2101,12 +2101,12 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>Viva: A Vida é uma Festa</t>
+          <t>Bastardos Inglórios</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>2017</t>
+          <t>2009</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
@@ -2123,12 +2123,12 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>O Barco: Inferno no Mar</t>
+          <t>Viva: A Vida é uma Festa</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>1981</t>
+          <t>2017</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
@@ -2145,12 +2145,12 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>Bastardos Inglórios</t>
+          <t>O Barco: Inferno no Mar</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>2009</t>
+          <t>1981</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
@@ -2255,12 +2255,12 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>Toy Story 3</t>
+          <t>Your Name.</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>2010</t>
+          <t>2016</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
@@ -2299,12 +2299,12 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>Your Name.</t>
+          <t>Toy Story 3</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>2016</t>
+          <t>2010</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
@@ -2365,12 +2365,12 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>Star Wars, Episódio VI: O Retorno do Jedi</t>
+          <t>Céu E Inferno</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>1983</t>
+          <t>1963</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
@@ -2387,12 +2387,12 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>2001: Uma Odisséia no Espaço</t>
+          <t>Star Wars, Episódio VI: O Retorno do Jedi</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>1968</t>
+          <t>1983</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
@@ -2409,12 +2409,12 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>Brilho Eterno de uma Mente sem Lembranças</t>
+          <t>2001: Uma Odisséia no Espaço</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>2004</t>
+          <t>1968</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
@@ -2431,12 +2431,12 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>Cães de Aluguel</t>
+          <t>Brilho Eterno de uma Mente sem Lembranças</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>1992</t>
+          <t>2004</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
@@ -2453,12 +2453,12 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>Céu E Inferno</t>
+          <t>Cães de Aluguel</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>1963</t>
+          <t>1992</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
@@ -2497,12 +2497,12 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>Cidadão Kane</t>
+          <t>A Caça</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>1941</t>
+          <t>2012</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
@@ -2541,12 +2541,12 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>A Caça</t>
+          <t>Cidadão Kane</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>2012</t>
+          <t>1941</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
@@ -2607,12 +2607,12 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>Um Corpo que Cai</t>
+          <t>Vá e Veja</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>1958</t>
+          <t>1985</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
@@ -2629,12 +2629,12 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>O Fabuloso Destino de Amélie Poulain</t>
+          <t>Um Corpo que Cai</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>2001</t>
+          <t>1958</t>
         </is>
       </c>
       <c r="D101" t="inlineStr">
@@ -2651,12 +2651,12 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>Laranja Mecânica</t>
+          <t>O Fabuloso Destino de Amélie Poulain</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>1971</t>
+          <t>2001</t>
         </is>
       </c>
       <c r="D102" t="inlineStr">
@@ -2673,12 +2673,12 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>Vá e Veja</t>
+          <t>Laranja Mecânica</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>1985</t>
+          <t>1971</t>
         </is>
       </c>
       <c r="D103" t="inlineStr">
@@ -2695,12 +2695,12 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>Nascido para Matar</t>
+          <t>Pacto de Sangue</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>1987</t>
+          <t>1944</t>
         </is>
       </c>
       <c r="D104" t="inlineStr">
@@ -2717,12 +2717,12 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>Pacto de Sangue</t>
+          <t>Nascido para Matar</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>1944</t>
+          <t>1987</t>
         </is>
       </c>
       <c r="D105" t="inlineStr">
@@ -2761,12 +2761,12 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>Scarface</t>
+          <t>Viver</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>1983</t>
+          <t>1952</t>
         </is>
       </c>
       <c r="D107" t="inlineStr">
@@ -2783,12 +2783,12 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>Viver</t>
+          <t>Scarface</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>1952</t>
+          <t>1983</t>
         </is>
       </c>
       <c r="D108" t="inlineStr">
@@ -2871,12 +2871,12 @@
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>Up: Altas Aventuras</t>
+          <t>Fogo Contra Fogo</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>2009</t>
+          <t>1995</t>
         </is>
       </c>
       <c r="D112" t="inlineStr">
@@ -2893,12 +2893,12 @@
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>Los Angeles: Cidade Proibida</t>
+          <t>Up: Altas Aventuras</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>1997</t>
+          <t>2009</t>
         </is>
       </c>
       <c r="D113" t="inlineStr">
@@ -2915,12 +2915,12 @@
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>Fogo Contra Fogo</t>
+          <t>Los Angeles: Cidade Proibida</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>1995</t>
+          <t>1997</t>
         </is>
       </c>
       <c r="D114" t="inlineStr">
@@ -2937,12 +2937,12 @@
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>Metrópolis</t>
+          <t>Incêndios</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>1927</t>
+          <t>2010</t>
         </is>
       </c>
       <c r="D115" t="inlineStr">
@@ -2959,12 +2959,12 @@
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>Hamilton</t>
+          <t>Metrópolis</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>2020</t>
+          <t>1927</t>
         </is>
       </c>
       <c r="D116" t="inlineStr">
@@ -3003,12 +3003,12 @@
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>Snatch: Porcos e Diamantes</t>
+          <t>Hamilton</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>2000</t>
+          <t>2020</t>
         </is>
       </c>
       <c r="D118" t="inlineStr">
@@ -3047,12 +3047,12 @@
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>Incêndios</t>
+          <t>Snatch: Porcos e Diamantes</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>2010</t>
+          <t>2000</t>
         </is>
       </c>
       <c r="D120" t="inlineStr">
@@ -3179,12 +3179,12 @@
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>Homem-Aranha: Sem Volta para Casa</t>
+          <t>Por uns Dólares a Mais</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>2021</t>
+          <t>1965</t>
         </is>
       </c>
       <c r="D126" t="inlineStr">
@@ -3201,12 +3201,12 @@
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>Por uns Dólares a Mais</t>
+          <t>Batman Begins</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>1965</t>
+          <t>2005</t>
         </is>
       </c>
       <c r="D127" t="inlineStr">
@@ -3223,12 +3223,12 @@
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>Batman Begins</t>
+          <t>Dangal</t>
         </is>
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>2005</t>
+          <t>2016</t>
         </is>
       </c>
       <c r="D128" t="inlineStr">
@@ -3245,12 +3245,12 @@
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>Dangal</t>
+          <t>O Garoto</t>
         </is>
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>2016</t>
+          <t>1921</t>
         </is>
       </c>
       <c r="D129" t="inlineStr">
@@ -3267,12 +3267,12 @@
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>O Garoto</t>
+          <t>Quanto Mais Quente Melhor</t>
         </is>
       </c>
       <c r="C130" t="inlineStr">
         <is>
-          <t>1921</t>
+          <t>1959</t>
         </is>
       </c>
       <c r="D130" t="inlineStr">
@@ -3289,12 +3289,12 @@
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>Quanto Mais Quente Melhor</t>
+          <t>A Malvada</t>
         </is>
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>1959</t>
+          <t>1950</t>
         </is>
       </c>
       <c r="D131" t="inlineStr">
@@ -3333,12 +3333,12 @@
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>A Malvada</t>
+          <t>Green Book: O Guia</t>
         </is>
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>1950</t>
+          <t>2018</t>
         </is>
       </c>
       <c r="D133" t="inlineStr">
@@ -3355,12 +3355,12 @@
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>Green Book: O Guia</t>
+          <t>O Lobo de Wall Street</t>
         </is>
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>2018</t>
+          <t>2013</t>
         </is>
       </c>
       <c r="D134" t="inlineStr">
@@ -3377,12 +3377,12 @@
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>O Lobo de Wall Street</t>
+          <t>Julgamento em Nuremberg</t>
         </is>
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>2013</t>
+          <t>1961</t>
         </is>
       </c>
       <c r="D135" t="inlineStr">
@@ -3399,12 +3399,12 @@
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>Julgamento em Nuremberg</t>
+          <t>Homem-Aranha: Sem Volta para Casa</t>
         </is>
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t>1961</t>
+          <t>2021</t>
         </is>
       </c>
       <c r="D136" t="inlineStr">
@@ -3421,12 +3421,12 @@
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>Os Imperdoáveis</t>
+          <t>Ran</t>
         </is>
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>1992</t>
+          <t>1985</t>
         </is>
       </c>
       <c r="D137" t="inlineStr">
@@ -3443,12 +3443,12 @@
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>Ran</t>
+          <t>Cassino</t>
         </is>
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>1985</t>
+          <t>1995</t>
         </is>
       </c>
       <c r="D138" t="inlineStr">
@@ -3465,12 +3465,12 @@
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>Cassino</t>
+          <t>Os Imperdoáveis</t>
         </is>
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>1995</t>
+          <t>1992</t>
         </is>
       </c>
       <c r="D139" t="inlineStr">
@@ -3531,12 +3531,12 @@
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>O Sexto Sentido</t>
+          <t>O Show de Truman: O Show da Vida</t>
         </is>
       </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t>1999</t>
+          <t>1998</t>
         </is>
       </c>
       <c r="D142" t="inlineStr">
@@ -3553,12 +3553,12 @@
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>Uma Mente Brilhante</t>
+          <t>O Sexto Sentido</t>
         </is>
       </c>
       <c r="C143" t="inlineStr">
         <is>
-          <t>2001</t>
+          <t>1999</t>
         </is>
       </c>
       <c r="D143" t="inlineStr">
@@ -3575,12 +3575,12 @@
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>O Show de Truman: O Show da Vida</t>
+          <t>Uma Mente Brilhante</t>
         </is>
       </c>
       <c r="C144" t="inlineStr">
         <is>
-          <t>1998</t>
+          <t>2001</t>
         </is>
       </c>
       <c r="D144" t="inlineStr">
@@ -3607,7 +3607,7 @@
       </c>
       <c r="D145" t="inlineStr">
         <is>
-          <t>8.2</t>
+          <t>8.1</t>
         </is>
       </c>
     </row>
@@ -3619,17 +3619,17 @@
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>Tudo em Todo Lugar ao Mesmo Tempo</t>
+          <t>Yojimbo, o Guarda-Costas</t>
         </is>
       </c>
       <c r="C146" t="inlineStr">
         <is>
-          <t>2022</t>
+          <t>1961</t>
         </is>
       </c>
       <c r="D146" t="inlineStr">
         <is>
-          <t>8.2</t>
+          <t>8.1</t>
         </is>
       </c>
     </row>
@@ -3641,12 +3641,12 @@
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>Yojimbo, o Guarda-Costas</t>
+          <t>O Tesouro da Sierra Madre</t>
         </is>
       </c>
       <c r="C147" t="inlineStr">
         <is>
-          <t>1961</t>
+          <t>1948</t>
         </is>
       </c>
       <c r="D147" t="inlineStr">
@@ -3663,12 +3663,12 @@
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>O Tesouro da Sierra Madre</t>
+          <t>Ilha do Medo</t>
         </is>
       </c>
       <c r="C148" t="inlineStr">
         <is>
-          <t>1948</t>
+          <t>2010</t>
         </is>
       </c>
       <c r="D148" t="inlineStr">
@@ -3685,12 +3685,12 @@
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>Ilha do Medo</t>
+          <t>Jurassic Park</t>
         </is>
       </c>
       <c r="C149" t="inlineStr">
         <is>
-          <t>2010</t>
+          <t>1993</t>
         </is>
       </c>
       <c r="D149" t="inlineStr">
@@ -3729,12 +3729,12 @@
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>Jurassic Park</t>
+          <t>Fugindo do Inferno</t>
         </is>
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>1993</t>
+          <t>1963</t>
         </is>
       </c>
       <c r="D151" t="inlineStr">
@@ -3751,12 +3751,12 @@
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>Fugindo do Inferno</t>
+          <t>Kill Bill: Volume 1</t>
         </is>
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>1963</t>
+          <t>2003</t>
         </is>
       </c>
       <c r="D152" t="inlineStr">
@@ -3773,12 +3773,12 @@
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>Kill Bill: Volume 1</t>
+          <t>Onde os Fracos Não Têm Vez</t>
         </is>
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>2003</t>
+          <t>2007</t>
         </is>
       </c>
       <c r="D153" t="inlineStr">
@@ -3795,12 +3795,12 @@
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>Onde os Fracos Não Têm Vez</t>
+          <t>Procurando Nemo</t>
         </is>
       </c>
       <c r="C154" t="inlineStr">
         <is>
-          <t>2007</t>
+          <t>2003</t>
         </is>
       </c>
       <c r="D154" t="inlineStr">
@@ -3817,12 +3817,12 @@
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>Procurando Nemo</t>
+          <t>O Homem Elefante</t>
         </is>
       </c>
       <c r="C155" t="inlineStr">
         <is>
-          <t>2003</t>
+          <t>1980</t>
         </is>
       </c>
       <c r="D155" t="inlineStr">
@@ -3839,12 +3839,12 @@
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>O Homem Elefante</t>
+          <t>Chinatown</t>
         </is>
       </c>
       <c r="C156" t="inlineStr">
         <is>
-          <t>1980</t>
+          <t>1974</t>
         </is>
       </c>
       <c r="D156" t="inlineStr">
@@ -3861,12 +3861,12 @@
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>Chinatown</t>
+          <t>Touro Indomável</t>
         </is>
       </c>
       <c r="C157" t="inlineStr">
         <is>
-          <t>1974</t>
+          <t>1980</t>
         </is>
       </c>
       <c r="D157" t="inlineStr">
@@ -3883,12 +3883,12 @@
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>Touro Indomável</t>
+          <t>O Enigma de Outro Mundo</t>
         </is>
       </c>
       <c r="C158" t="inlineStr">
         <is>
-          <t>1980</t>
+          <t>1982</t>
         </is>
       </c>
       <c r="D158" t="inlineStr">
@@ -3949,12 +3949,12 @@
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>O Enigma de Outro Mundo</t>
+          <t>Divertida Mente</t>
         </is>
       </c>
       <c r="C161" t="inlineStr">
         <is>
-          <t>1982</t>
+          <t>2015</t>
         </is>
       </c>
       <c r="D161" t="inlineStr">
@@ -3971,12 +3971,12 @@
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>Divertida Mente</t>
+          <t>Jogos, Trapaças e Dois Canos Fumegantes</t>
         </is>
       </c>
       <c r="C162" t="inlineStr">
         <is>
-          <t>2015</t>
+          <t>1998</t>
         </is>
       </c>
       <c r="D162" t="inlineStr">
@@ -3993,12 +3993,12 @@
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>Jogos, Trapaças e Dois Canos Fumegantes</t>
+          <t>Disque M para Matar</t>
         </is>
       </c>
       <c r="C163" t="inlineStr">
         <is>
-          <t>1998</t>
+          <t>1954</t>
         </is>
       </c>
       <c r="D163" t="inlineStr">
@@ -4015,12 +4015,12 @@
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>Disque M para Matar</t>
+          <t>O Segredo dos Seus Olhos</t>
         </is>
       </c>
       <c r="C164" t="inlineStr">
         <is>
-          <t>1954</t>
+          <t>2009</t>
         </is>
       </c>
       <c r="D164" t="inlineStr">
@@ -4037,12 +4037,12 @@
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>O Segredo dos Seus Olhos</t>
+          <t>O Castelo Animado</t>
         </is>
       </c>
       <c r="C165" t="inlineStr">
         <is>
-          <t>2009</t>
+          <t>2004</t>
         </is>
       </c>
       <c r="D165" t="inlineStr">
@@ -4081,12 +4081,12 @@
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>O Castelo Animado</t>
+          <t>Três Anúncios para um Crime</t>
         </is>
       </c>
       <c r="C167" t="inlineStr">
         <is>
-          <t>2004</t>
+          <t>2017</t>
         </is>
       </c>
       <c r="D167" t="inlineStr">
@@ -4103,12 +4103,12 @@
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>Três Anúncios para um Crime</t>
+          <t>Trainspotting: Sem Limites</t>
         </is>
       </c>
       <c r="C168" t="inlineStr">
         <is>
-          <t>2017</t>
+          <t>1996</t>
         </is>
       </c>
       <c r="D168" t="inlineStr">
@@ -4125,12 +4125,12 @@
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>Trainspotting: Sem Limites</t>
+          <t>Guerreiro</t>
         </is>
       </c>
       <c r="C169" t="inlineStr">
         <is>
-          <t>1996</t>
+          <t>2011</t>
         </is>
       </c>
       <c r="D169" t="inlineStr">
@@ -4169,12 +4169,12 @@
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>Guerreiro</t>
+          <t>Fargo: Uma Comédia de Erros</t>
         </is>
       </c>
       <c r="C171" t="inlineStr">
         <is>
-          <t>2011</t>
+          <t>1996</t>
         </is>
       </c>
       <c r="D171" t="inlineStr">
@@ -4191,12 +4191,12 @@
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>Fargo: Uma Comédia de Erros</t>
+          <t>Os Suspeitos</t>
         </is>
       </c>
       <c r="C172" t="inlineStr">
         <is>
-          <t>1996</t>
+          <t>2013</t>
         </is>
       </c>
       <c r="D172" t="inlineStr">
@@ -4213,12 +4213,12 @@
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>Os Suspeitos</t>
+          <t>Meu Amigo Totoro</t>
         </is>
       </c>
       <c r="C173" t="inlineStr">
         <is>
-          <t>2013</t>
+          <t>1988</t>
         </is>
       </c>
       <c r="D173" t="inlineStr">
@@ -4235,12 +4235,12 @@
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>Meu Amigo Totoro</t>
+          <t>Menina de Ouro</t>
         </is>
       </c>
       <c r="C174" t="inlineStr">
         <is>
-          <t>1988</t>
+          <t>2004</t>
         </is>
       </c>
       <c r="D174" t="inlineStr">
@@ -4257,12 +4257,12 @@
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>Menina de Ouro</t>
+          <t>Prenda-me se for Capaz</t>
         </is>
       </c>
       <c r="C175" t="inlineStr">
         <is>
-          <t>2004</t>
+          <t>2002</t>
         </is>
       </c>
       <c r="D175" t="inlineStr">
@@ -4301,12 +4301,12 @@
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t>Prenda-me se for Capaz</t>
+          <t>Blade Runner: O Caçador de Androides</t>
         </is>
       </c>
       <c r="C177" t="inlineStr">
         <is>
-          <t>2002</t>
+          <t>1982</t>
         </is>
       </c>
       <c r="D177" t="inlineStr">
@@ -4323,12 +4323,12 @@
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>Blade Runner: O Caçador de Androides</t>
+          <t>Sindicato de Ladrões</t>
         </is>
       </c>
       <c r="C178" t="inlineStr">
         <is>
-          <t>1982</t>
+          <t>1954</t>
         </is>
       </c>
       <c r="D178" t="inlineStr">
@@ -4345,12 +4345,12 @@
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>Sindicato de Ladrões</t>
+          <t>Filhos do Paraíso</t>
         </is>
       </c>
       <c r="C179" t="inlineStr">
         <is>
-          <t>1954</t>
+          <t>1997</t>
         </is>
       </c>
       <c r="D179" t="inlineStr">
@@ -4389,12 +4389,12 @@
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>Filhos do Paraíso</t>
+          <t>Antes do Amanhecer</t>
         </is>
       </c>
       <c r="C181" t="inlineStr">
         <is>
-          <t>1997</t>
+          <t>1995</t>
         </is>
       </c>
       <c r="D181" t="inlineStr">
@@ -4455,12 +4455,12 @@
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>A General</t>
+          <t>Morangos Silvestres</t>
         </is>
       </c>
       <c r="C184" t="inlineStr">
         <is>
-          <t>1926</t>
+          <t>1957</t>
         </is>
       </c>
       <c r="D184" t="inlineStr">
@@ -4477,12 +4477,12 @@
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>Antes do Amanhecer</t>
+          <t>Harry Potter e as Relíquias da Morte - Parte 2</t>
         </is>
       </c>
       <c r="C185" t="inlineStr">
         <is>
-          <t>1995</t>
+          <t>2011</t>
         </is>
       </c>
       <c r="D185" t="inlineStr">
@@ -4499,12 +4499,12 @@
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>Morangos Silvestres</t>
+          <t>Garota Exemplar</t>
         </is>
       </c>
       <c r="C186" t="inlineStr">
         <is>
-          <t>1957</t>
+          <t>2014</t>
         </is>
       </c>
       <c r="D186" t="inlineStr">
@@ -4521,12 +4521,12 @@
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>Garota Exemplar</t>
+          <t>A General</t>
         </is>
       </c>
       <c r="C187" t="inlineStr">
         <is>
-          <t>2014</t>
+          <t>1926</t>
         </is>
       </c>
       <c r="D187" t="inlineStr">
@@ -4543,12 +4543,12 @@
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>Harry Potter e as Relíquias da Morte - Parte 2</t>
+          <t>O Franco Atirador</t>
         </is>
       </c>
       <c r="C188" t="inlineStr">
         <is>
-          <t>2011</t>
+          <t>1978</t>
         </is>
       </c>
       <c r="D188" t="inlineStr">
@@ -4565,12 +4565,12 @@
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>O Franco Atirador</t>
+          <t>Em Nome do Pai</t>
         </is>
       </c>
       <c r="C189" t="inlineStr">
         <is>
-          <t>1978</t>
+          <t>1993</t>
         </is>
       </c>
       <c r="D189" t="inlineStr">
@@ -4587,12 +4587,12 @@
       </c>
       <c r="B190" t="inlineStr">
         <is>
-          <t>Em Nome do Pai</t>
+          <t>O Grande Hotel Budapeste</t>
         </is>
       </c>
       <c r="C190" t="inlineStr">
         <is>
-          <t>1993</t>
+          <t>2014</t>
         </is>
       </c>
       <c r="D190" t="inlineStr">
@@ -4609,12 +4609,12 @@
       </c>
       <c r="B191" t="inlineStr">
         <is>
-          <t>O Grande Hotel Budapeste</t>
+          <t>Barry Lyndon</t>
         </is>
       </c>
       <c r="C191" t="inlineStr">
         <is>
-          <t>2014</t>
+          <t>1975</t>
         </is>
       </c>
       <c r="D191" t="inlineStr">
@@ -4631,12 +4631,12 @@
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>A Mulher Faz o Homem</t>
+          <t>O Salário do Medo</t>
         </is>
       </c>
       <c r="C192" t="inlineStr">
         <is>
-          <t>1939</t>
+          <t>1953</t>
         </is>
       </c>
       <c r="D192" t="inlineStr">
@@ -4653,12 +4653,12 @@
       </c>
       <c r="B193" t="inlineStr">
         <is>
-          <t>O Salário do Medo</t>
+          <t>A Mulher Faz o Homem</t>
         </is>
       </c>
       <c r="C193" t="inlineStr">
         <is>
-          <t>1953</t>
+          <t>1939</t>
         </is>
       </c>
       <c r="D193" t="inlineStr">
@@ -4675,12 +4675,12 @@
       </c>
       <c r="B194" t="inlineStr">
         <is>
-          <t>Barry Lyndon</t>
+          <t>Bancando o Águia</t>
         </is>
       </c>
       <c r="C194" t="inlineStr">
         <is>
-          <t>1975</t>
+          <t>1924</t>
         </is>
       </c>
       <c r="D194" t="inlineStr">
@@ -4697,12 +4697,12 @@
       </c>
       <c r="B195" t="inlineStr">
         <is>
-          <t>Bancando o Águia</t>
+          <t>Até o Último Homem</t>
         </is>
       </c>
       <c r="C195" t="inlineStr">
         <is>
-          <t>1924</t>
+          <t>2016</t>
         </is>
       </c>
       <c r="D195" t="inlineStr">
@@ -4763,12 +4763,12 @@
       </c>
       <c r="B198" t="inlineStr">
         <is>
-          <t>Até o Último Homem</t>
+          <t>Relatos Selvagens</t>
         </is>
       </c>
       <c r="C198" t="inlineStr">
         <is>
-          <t>2016</t>
+          <t>2014</t>
         </is>
       </c>
       <c r="D198" t="inlineStr">
@@ -4785,12 +4785,12 @@
       </c>
       <c r="B199" t="inlineStr">
         <is>
-          <t>O Quarto de Jack</t>
+          <t>O Sétimo Selo</t>
         </is>
       </c>
       <c r="C199" t="inlineStr">
         <is>
-          <t>2015</t>
+          <t>1957</t>
         </is>
       </c>
       <c r="D199" t="inlineStr">
@@ -4807,12 +4807,12 @@
       </c>
       <c r="B200" t="inlineStr">
         <is>
-          <t>O Sétimo Selo</t>
+          <t>O Quarto de Jack</t>
         </is>
       </c>
       <c r="C200" t="inlineStr">
         <is>
-          <t>1957</t>
+          <t>2015</t>
         </is>
       </c>
       <c r="D200" t="inlineStr">
@@ -4829,12 +4829,12 @@
       </c>
       <c r="B201" t="inlineStr">
         <is>
-          <t>Relatos Selvagens</t>
+          <t>Tudo em Todo Lugar ao Mesmo Tempo</t>
         </is>
       </c>
       <c r="C201" t="inlineStr">
         <is>
-          <t>2014</t>
+          <t>2022</t>
         </is>
       </c>
       <c r="D201" t="inlineStr">
@@ -4851,12 +4851,12 @@
       </c>
       <c r="B202" t="inlineStr">
         <is>
-          <t>O Grande Lebowski</t>
+          <t>Mad Max: Estrada da Fúria</t>
         </is>
       </c>
       <c r="C202" t="inlineStr">
         <is>
-          <t>1998</t>
+          <t>2015</t>
         </is>
       </c>
       <c r="D202" t="inlineStr">
@@ -4873,12 +4873,12 @@
       </c>
       <c r="B203" t="inlineStr">
         <is>
-          <t>Mad Max: Estrada da Fúria</t>
+          <t>Como Treinar o Seu Dragão</t>
         </is>
       </c>
       <c r="C203" t="inlineStr">
         <is>
-          <t>2015</t>
+          <t>2010</t>
         </is>
       </c>
       <c r="D203" t="inlineStr">
@@ -4895,12 +4895,12 @@
       </c>
       <c r="B204" t="inlineStr">
         <is>
-          <t>Como Treinar o Seu Dragão</t>
+          <t>O Grande Lebowski</t>
         </is>
       </c>
       <c r="C204" t="inlineStr">
         <is>
-          <t>2010</t>
+          <t>1998</t>
         </is>
       </c>
       <c r="D204" t="inlineStr">
@@ -4939,12 +4939,12 @@
       </c>
       <c r="B206" t="inlineStr">
         <is>
-          <t>Monstros S.A.</t>
+          <t>Tubarão</t>
         </is>
       </c>
       <c r="C206" t="inlineStr">
         <is>
-          <t>2001</t>
+          <t>1975</t>
         </is>
       </c>
       <c r="D206" t="inlineStr">
@@ -4961,12 +4961,12 @@
       </c>
       <c r="B207" t="inlineStr">
         <is>
-          <t>Tubarão</t>
+          <t>Monstros S.A.</t>
         </is>
       </c>
       <c r="C207" t="inlineStr">
         <is>
-          <t>1975</t>
+          <t>2001</t>
         </is>
       </c>
       <c r="D207" t="inlineStr">
@@ -4983,12 +4983,12 @@
       </c>
       <c r="B208" t="inlineStr">
         <is>
-          <t>O Martírio de Joana D'Arc</t>
+          <t>Era uma Vez em Tóquio</t>
         </is>
       </c>
       <c r="C208" t="inlineStr">
         <is>
-          <t>1928</t>
+          <t>1953</t>
         </is>
       </c>
       <c r="D208" t="inlineStr">
@@ -5027,12 +5027,12 @@
       </c>
       <c r="B210" t="inlineStr">
         <is>
-          <t>Hotel Ruanda</t>
+          <t>O Martírio de Joana D'Arc</t>
         </is>
       </c>
       <c r="C210" t="inlineStr">
         <is>
-          <t>2004</t>
+          <t>1928</t>
         </is>
       </c>
       <c r="D210" t="inlineStr">
@@ -5049,12 +5049,12 @@
       </c>
       <c r="B211" t="inlineStr">
         <is>
-          <t>Era uma Vez em Tóquio</t>
+          <t>Hotel Ruanda</t>
         </is>
       </c>
       <c r="C211" t="inlineStr">
         <is>
-          <t>1953</t>
+          <t>2004</t>
         </is>
       </c>
       <c r="D211" t="inlineStr">
@@ -5071,12 +5071,12 @@
       </c>
       <c r="B212" t="inlineStr">
         <is>
-          <t>A Canção da Estrada</t>
+          <t>Rocky: Um Lutador</t>
         </is>
       </c>
       <c r="C212" t="inlineStr">
         <is>
-          <t>1955</t>
+          <t>1976</t>
         </is>
       </c>
       <c r="D212" t="inlineStr">
@@ -5093,12 +5093,12 @@
       </c>
       <c r="B213" t="inlineStr">
         <is>
-          <t>Rocky: Um Lutador</t>
+          <t>Ford vs Ferrari</t>
         </is>
       </c>
       <c r="C213" t="inlineStr">
         <is>
-          <t>1976</t>
+          <t>2019</t>
         </is>
       </c>
       <c r="D213" t="inlineStr">
@@ -5137,12 +5137,12 @@
       </c>
       <c r="B215" t="inlineStr">
         <is>
-          <t>Ford vs Ferrari</t>
+          <t>A Canção da Estrada</t>
         </is>
       </c>
       <c r="C215" t="inlineStr">
         <is>
-          <t>2019</t>
+          <t>1955</t>
         </is>
       </c>
       <c r="D215" t="inlineStr">
@@ -5247,12 +5247,12 @@
       </c>
       <c r="B220" t="inlineStr">
         <is>
-          <t>Rede de Intrigas</t>
+          <t>Logan</t>
         </is>
       </c>
       <c r="C220" t="inlineStr">
         <is>
-          <t>1976</t>
+          <t>2017</t>
         </is>
       </c>
       <c r="D220" t="inlineStr">
@@ -5269,12 +5269,12 @@
       </c>
       <c r="B221" t="inlineStr">
         <is>
-          <t>Na Natureza Selvagem</t>
+          <t>Rede de Intrigas</t>
         </is>
       </c>
       <c r="C221" t="inlineStr">
         <is>
-          <t>2007</t>
+          <t>1976</t>
         </is>
       </c>
       <c r="D221" t="inlineStr">
@@ -5291,12 +5291,12 @@
       </c>
       <c r="B222" t="inlineStr">
         <is>
-          <t>Logan</t>
+          <t>Ratatouille</t>
         </is>
       </c>
       <c r="C222" t="inlineStr">
         <is>
-          <t>2017</t>
+          <t>2007</t>
         </is>
       </c>
       <c r="D222" t="inlineStr">
@@ -5313,12 +5313,12 @@
       </c>
       <c r="B223" t="inlineStr">
         <is>
-          <t>O Mágico de Oz</t>
+          <t>Na Natureza Selvagem</t>
         </is>
       </c>
       <c r="C223" t="inlineStr">
         <is>
-          <t>1939</t>
+          <t>2007</t>
         </is>
       </c>
       <c r="D223" t="inlineStr">
@@ -5335,12 +5335,12 @@
       </c>
       <c r="B224" t="inlineStr">
         <is>
-          <t>Ratatouille</t>
+          <t>O Mágico de Oz</t>
         </is>
       </c>
       <c r="C224" t="inlineStr">
         <is>
-          <t>2007</t>
+          <t>1939</t>
         </is>
       </c>
       <c r="D224" t="inlineStr">
@@ -5489,12 +5489,12 @@
       </c>
       <c r="B231" t="inlineStr">
         <is>
-          <t>Rebecca, a Mulher Inesquecível</t>
+          <t>A Batalha de Argel</t>
         </is>
       </c>
       <c r="C231" t="inlineStr">
         <is>
-          <t>1940</t>
+          <t>1966</t>
         </is>
       </c>
       <c r="D231" t="inlineStr">
@@ -5533,12 +5533,12 @@
       </c>
       <c r="B233" t="inlineStr">
         <is>
-          <t>A Batalha de Argel</t>
+          <t>Rebecca, a Mulher Inesquecível</t>
         </is>
       </c>
       <c r="C233" t="inlineStr">
         <is>
-          <t>1966</t>
+          <t>1940</t>
         </is>
       </c>
       <c r="D233" t="inlineStr">
@@ -5643,12 +5643,12 @@
       </c>
       <c r="B238" t="inlineStr">
         <is>
-          <t>O Ódio</t>
+          <t>Jai Bhim</t>
         </is>
       </c>
       <c r="C238" t="inlineStr">
         <is>
-          <t>1995</t>
+          <t>2021</t>
         </is>
       </c>
       <c r="D238" t="inlineStr">
@@ -5665,12 +5665,12 @@
       </c>
       <c r="B239" t="inlineStr">
         <is>
-          <t>Os Incompreendidos</t>
+          <t>O Ódio</t>
         </is>
       </c>
       <c r="C239" t="inlineStr">
         <is>
-          <t>1959</t>
+          <t>1995</t>
         </is>
       </c>
       <c r="D239" t="inlineStr">
@@ -5687,12 +5687,12 @@
       </c>
       <c r="B240" t="inlineStr">
         <is>
-          <t>Quando Duas Mulheres Pecam</t>
+          <t>Meu Pai e Meu Filho</t>
         </is>
       </c>
       <c r="C240" t="inlineStr">
         <is>
-          <t>1966</t>
+          <t>2005</t>
         </is>
       </c>
       <c r="D240" t="inlineStr">
@@ -5709,12 +5709,12 @@
       </c>
       <c r="B241" t="inlineStr">
         <is>
-          <t>Meu Pai e Meu Filho</t>
+          <t>Os Incompreendidos</t>
         </is>
       </c>
       <c r="C241" t="inlineStr">
         <is>
-          <t>2005</t>
+          <t>1959</t>
         </is>
       </c>
       <c r="D241" t="inlineStr">
@@ -5731,12 +5731,12 @@
       </c>
       <c r="B242" t="inlineStr">
         <is>
-          <t>A Vida de Brian</t>
+          <t>Quando Duas Mulheres Pecam</t>
         </is>
       </c>
       <c r="C242" t="inlineStr">
         <is>
-          <t>1979</t>
+          <t>1966</t>
         </is>
       </c>
       <c r="D242" t="inlineStr">
@@ -5775,12 +5775,12 @@
       </c>
       <c r="B244" t="inlineStr">
         <is>
-          <t>A Noviça Rebelde</t>
+          <t>A Vida de Brian</t>
         </is>
       </c>
       <c r="C244" t="inlineStr">
         <is>
-          <t>1965</t>
+          <t>1979</t>
         </is>
       </c>
       <c r="D244" t="inlineStr">
@@ -5797,12 +5797,12 @@
       </c>
       <c r="B245" t="inlineStr">
         <is>
-          <t>Dersu Uzala</t>
+          <t>A Noviça Rebelde</t>
         </is>
       </c>
       <c r="C245" t="inlineStr">
         <is>
-          <t>1975</t>
+          <t>1965</t>
         </is>
       </c>
       <c r="D245" t="inlineStr">
@@ -5841,12 +5841,12 @@
       </c>
       <c r="B247" t="inlineStr">
         <is>
-          <t>Jai Bhim</t>
+          <t>Dersu Uzala</t>
         </is>
       </c>
       <c r="C247" t="inlineStr">
         <is>
-          <t>2021</t>
+          <t>1975</t>
         </is>
       </c>
       <c r="D247" t="inlineStr">
@@ -5929,12 +5929,12 @@
       </c>
       <c r="B251" t="inlineStr">
         <is>
-          <t>A Bela e a Fera</t>
+          <t>O Gigante de Ferro</t>
         </is>
       </c>
       <c r="C251" t="inlineStr">
         <is>
-          <t>1991</t>
+          <t>1999</t>
         </is>
       </c>
       <c r="D251" t="inlineStr">

</xml_diff>